<commit_message>
Session 11 Update with second strategy added
</commit_message>
<xml_diff>
--- a/data/KAHI_status_all.xlsx
+++ b/data/KAHI_status_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C42D5D-9AB8-A14F-9FBA-399F69F44025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC9CC8A-3300-194D-B402-AA00B34D6C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30560" yWindow="3640" windowWidth="28800" windowHeight="16420" xr2:uid="{3C916DE0-195B-2A4F-AB3E-F4618B8BB61D}"/>
   </bookViews>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D24135B-7C4E-9B44-8B3B-A592D6651794}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,6 +486,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>